<commit_message>
[FEATURE] Add 'OnlyActiveForLanguage' examples to the test scene and remove a few translations to test the import warning log.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/configuration.xlsx
+++ b/Assets/StreamingAssets/configuration.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -59,15 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">my.test.key3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DER GUTE TEXT 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THE GOOD TEXT 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">退出</t>
   </si>
 </sst>
 </file>
@@ -234,20 +225,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W221"/>
+  <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -378,15 +369,9 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>

</xml_diff>

<commit_message>
[FEATURE] Improve example scene to test the newest features.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/configuration.xlsx
+++ b/Assets/StreamingAssets/configuration.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -31,34 +31,55 @@
     <t xml:space="preserve">English</t>
   </si>
   <si>
-    <t xml:space="preserve">Chinese</t>
+    <t xml:space="preserve">Simplified Chinese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korean</t>
   </si>
   <si>
     <t xml:space="preserve">my.test.key1</t>
   </si>
   <si>
-    <t xml:space="preserve">DER GUTE TEXT 1</t>
+    <t xml:space="preserve">Der gute Text 1</t>
   </si>
   <si>
-    <t xml:space="preserve">THE GOOD TEXT 1</t>
+    <t xml:space="preserve">The good text 1</t>
   </si>
   <si>
     <t xml:space="preserve">玩</t>
   </si>
   <si>
+    <t xml:space="preserve">등록하십시오 </t>
+  </si>
+  <si>
     <t xml:space="preserve">my.test.key2</t>
   </si>
   <si>
-    <t xml:space="preserve">DER GUTE TEXT 2</t>
+    <t xml:space="preserve">Der gute Text 2</t>
   </si>
   <si>
-    <t xml:space="preserve">THE GOOD TEXT 2</t>
+    <t xml:space="preserve">The good text 2</t>
   </si>
   <si>
     <t xml:space="preserve">设置</t>
   </si>
   <si>
+    <t xml:space="preserve">회의에서는 </t>
+  </si>
+  <si>
     <t xml:space="preserve">my.test.key3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der gute Text 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The good text 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">简化字总表</t>
+  </si>
+  <si>
+    <t xml:space="preserve">국제화와 </t>
   </si>
 </sst>
 </file>
@@ -69,7 +90,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -106,6 +127,12 @@
       <name val="Microsoft YaHei"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -163,7 +190,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -181,6 +208,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,16 +259,16 @@
   <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.93"/>
   </cols>
   <sheetData>
@@ -254,7 +285,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -301,18 +334,20 @@
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -334,18 +369,20 @@
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -367,12 +404,20 @@
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -481,9 +526,9 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -881,7 +926,7 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5"/>
+      <c r="A26" s="6"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="2"/>
@@ -906,7 +951,7 @@
       <c r="W26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5"/>
+      <c r="A27" s="6"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="2"/>
@@ -931,7 +976,7 @@
       <c r="W27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5"/>
+      <c r="A28" s="6"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -956,7 +1001,7 @@
       <c r="W28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5"/>
+      <c r="A29" s="6"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="2"/>
@@ -981,7 +1026,7 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5"/>
+      <c r="A30" s="6"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="2"/>
@@ -1006,7 +1051,7 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5"/>
+      <c r="A31" s="6"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="2"/>
@@ -1031,7 +1076,7 @@
       <c r="W31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5"/>
+      <c r="A32" s="6"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="2"/>
@@ -1056,7 +1101,7 @@
       <c r="W32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5"/>
+      <c r="A33" s="6"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="2"/>
@@ -1081,7 +1126,7 @@
       <c r="W33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5"/>
+      <c r="A34" s="6"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="2"/>
@@ -1586,7 +1631,7 @@
       <c r="W55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7"/>
+      <c r="A56" s="8"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="2"/>
@@ -1611,7 +1656,7 @@
       <c r="W56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5"/>
+      <c r="A57" s="6"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="2"/>
@@ -1636,7 +1681,7 @@
       <c r="W57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5"/>
+      <c r="A58" s="6"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="2"/>
@@ -1661,7 +1706,7 @@
       <c r="W58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5"/>
+      <c r="A59" s="6"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="2"/>
@@ -1686,7 +1731,7 @@
       <c r="W59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5"/>
+      <c r="A60" s="6"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="2"/>
@@ -1711,7 +1756,7 @@
       <c r="W60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5"/>
+      <c r="A61" s="6"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="2"/>
@@ -2311,7 +2356,7 @@
       <c r="W84" s="2"/>
     </row>
     <row r="85" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5"/>
+      <c r="A85" s="6"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="2"/>
@@ -2463,7 +2508,7 @@
     <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
-      <c r="C91" s="8"/>
+      <c r="C91" s="9"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
@@ -2886,7 +2931,7 @@
       <c r="W107" s="2"/>
     </row>
     <row r="108" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="9"/>
+      <c r="A108" s="10"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -2911,7 +2956,7 @@
       <c r="W108" s="2"/>
     </row>
     <row r="109" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="5"/>
+      <c r="A109" s="6"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="2"/>
@@ -2936,7 +2981,7 @@
       <c r="W109" s="2"/>
     </row>
     <row r="110" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="5"/>
+      <c r="A110" s="6"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="2"/>
@@ -2961,7 +3006,7 @@
       <c r="W110" s="2"/>
     </row>
     <row r="111" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="5"/>
+      <c r="A111" s="6"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="2"/>
@@ -2986,7 +3031,7 @@
       <c r="W111" s="2"/>
     </row>
     <row r="112" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="5"/>
+      <c r="A112" s="6"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="2"/>
@@ -3011,7 +3056,7 @@
       <c r="W112" s="2"/>
     </row>
     <row r="113" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="5"/>
+      <c r="A113" s="6"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="2"/>
@@ -3361,7 +3406,7 @@
       <c r="W126" s="2"/>
     </row>
     <row r="127" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="5"/>
+      <c r="A127" s="6"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="2"/>
@@ -3386,7 +3431,7 @@
       <c r="W127" s="2"/>
     </row>
     <row r="128" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="5"/>
+      <c r="A128" s="6"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="2"/>
@@ -3411,7 +3456,7 @@
       <c r="W128" s="2"/>
     </row>
     <row r="129" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="5"/>
+      <c r="A129" s="6"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="2"/>
@@ -3436,7 +3481,7 @@
       <c r="W129" s="2"/>
     </row>
     <row r="130" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="5"/>
+      <c r="A130" s="6"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
       <c r="D130" s="2"/>
@@ -3461,7 +3506,7 @@
       <c r="W130" s="2"/>
     </row>
     <row r="131" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="5"/>
+      <c r="A131" s="6"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="2"/>
@@ -3486,7 +3531,7 @@
       <c r="W131" s="2"/>
     </row>
     <row r="132" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="5"/>
+      <c r="A132" s="6"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
       <c r="D132" s="2"/>
@@ -3511,7 +3556,7 @@
       <c r="W132" s="2"/>
     </row>
     <row r="133" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="5"/>
+      <c r="A133" s="6"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
       <c r="D133" s="2"/>
@@ -3536,7 +3581,7 @@
       <c r="W133" s="2"/>
     </row>
     <row r="134" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="5"/>
+      <c r="A134" s="6"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
       <c r="D134" s="2"/>
@@ -4086,7 +4131,7 @@
       <c r="W155" s="2"/>
     </row>
     <row r="156" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A156" s="10"/>
+      <c r="A156" s="11"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
@@ -4136,7 +4181,7 @@
       <c r="W157" s="2"/>
     </row>
     <row r="158" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="5"/>
+      <c r="A158" s="6"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
       <c r="D158" s="2"/>

</xml_diff>

<commit_message>
[FEATURE] Test build with 'ClosedXML' and add example files for the localization differences.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/configuration.xlsx
+++ b/Assets/StreamingAssets/configuration.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">my.test.key3</t>
   </si>
   <si>
-    <t xml:space="preserve">Der gute Text 3</t>
+    <t xml:space="preserve">Der geänderte Text 3</t>
   </si>
   <si>
     <t xml:space="preserve">The good text 3</t>
@@ -81,6 +81,15 @@
   <si>
     <t xml:space="preserve">국제화와 </t>
   </si>
+  <si>
+    <t xml:space="preserve">my.test.key4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der gute Text 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The good text 4</t>
+  </si>
 </sst>
 </file>
 
@@ -90,7 +99,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -127,12 +136,6 @@
       <name val="Microsoft YaHei"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -190,7 +193,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,10 +211,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -259,13 +258,13 @@
   <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.31"/>
@@ -345,7 +344,7 @@
       <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="2"/>
@@ -380,7 +379,7 @@
       <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="2"/>
@@ -415,7 +414,7 @@
       <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="2"/>
@@ -438,6 +437,15 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -526,9 +534,9 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -926,7 +934,7 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
+      <c r="A26" s="5"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="2"/>
@@ -951,7 +959,7 @@
       <c r="W26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
+      <c r="A27" s="5"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="2"/>
@@ -976,7 +984,7 @@
       <c r="W27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
+      <c r="A28" s="5"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1001,7 +1009,7 @@
       <c r="W28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
+      <c r="A29" s="5"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="2"/>
@@ -1026,7 +1034,7 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6"/>
+      <c r="A30" s="5"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="2"/>
@@ -1051,7 +1059,7 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6"/>
+      <c r="A31" s="5"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="2"/>
@@ -1076,7 +1084,7 @@
       <c r="W31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6"/>
+      <c r="A32" s="5"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="2"/>
@@ -1101,7 +1109,7 @@
       <c r="W32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6"/>
+      <c r="A33" s="5"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="2"/>
@@ -1126,7 +1134,7 @@
       <c r="W33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6"/>
+      <c r="A34" s="5"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="2"/>
@@ -1631,7 +1639,7 @@
       <c r="W55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8"/>
+      <c r="A56" s="7"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="2"/>
@@ -1656,7 +1664,7 @@
       <c r="W56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6"/>
+      <c r="A57" s="5"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="2"/>
@@ -1681,7 +1689,7 @@
       <c r="W57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6"/>
+      <c r="A58" s="5"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="2"/>
@@ -1706,7 +1714,7 @@
       <c r="W58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="6"/>
+      <c r="A59" s="5"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="2"/>
@@ -1731,7 +1739,7 @@
       <c r="W59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="6"/>
+      <c r="A60" s="5"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="2"/>
@@ -1756,7 +1764,7 @@
       <c r="W60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="6"/>
+      <c r="A61" s="5"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="2"/>
@@ -2356,7 +2364,7 @@
       <c r="W84" s="2"/>
     </row>
     <row r="85" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="6"/>
+      <c r="A85" s="5"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="2"/>
@@ -2508,7 +2516,7 @@
     <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
-      <c r="C91" s="9"/>
+      <c r="C91" s="8"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
@@ -2931,7 +2939,7 @@
       <c r="W107" s="2"/>
     </row>
     <row r="108" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="10"/>
+      <c r="A108" s="9"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -2956,7 +2964,7 @@
       <c r="W108" s="2"/>
     </row>
     <row r="109" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="6"/>
+      <c r="A109" s="5"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="2"/>
@@ -2981,7 +2989,7 @@
       <c r="W109" s="2"/>
     </row>
     <row r="110" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="6"/>
+      <c r="A110" s="5"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="2"/>
@@ -3006,7 +3014,7 @@
       <c r="W110" s="2"/>
     </row>
     <row r="111" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="6"/>
+      <c r="A111" s="5"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="2"/>
@@ -3031,7 +3039,7 @@
       <c r="W111" s="2"/>
     </row>
     <row r="112" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="6"/>
+      <c r="A112" s="5"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="2"/>
@@ -3056,7 +3064,7 @@
       <c r="W112" s="2"/>
     </row>
     <row r="113" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="6"/>
+      <c r="A113" s="5"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="2"/>
@@ -3406,7 +3414,7 @@
       <c r="W126" s="2"/>
     </row>
     <row r="127" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="6"/>
+      <c r="A127" s="5"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="2"/>
@@ -3431,7 +3439,7 @@
       <c r="W127" s="2"/>
     </row>
     <row r="128" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="6"/>
+      <c r="A128" s="5"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="2"/>
@@ -3456,7 +3464,7 @@
       <c r="W128" s="2"/>
     </row>
     <row r="129" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="6"/>
+      <c r="A129" s="5"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="2"/>
@@ -3481,7 +3489,7 @@
       <c r="W129" s="2"/>
     </row>
     <row r="130" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="6"/>
+      <c r="A130" s="5"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
       <c r="D130" s="2"/>
@@ -3506,7 +3514,7 @@
       <c r="W130" s="2"/>
     </row>
     <row r="131" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="6"/>
+      <c r="A131" s="5"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="2"/>
@@ -3531,7 +3539,7 @@
       <c r="W131" s="2"/>
     </row>
     <row r="132" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="6"/>
+      <c r="A132" s="5"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
       <c r="D132" s="2"/>
@@ -3556,7 +3564,7 @@
       <c r="W132" s="2"/>
     </row>
     <row r="133" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="6"/>
+      <c r="A133" s="5"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
       <c r="D133" s="2"/>
@@ -3581,7 +3589,7 @@
       <c r="W133" s="2"/>
     </row>
     <row r="134" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="6"/>
+      <c r="A134" s="5"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
       <c r="D134" s="2"/>
@@ -4131,7 +4139,7 @@
       <c r="W155" s="2"/>
     </row>
     <row r="156" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A156" s="11"/>
+      <c r="A156" s="10"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
@@ -4181,7 +4189,7 @@
       <c r="W157" s="2"/>
     </row>
     <row r="158" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="6"/>
+      <c r="A158" s="5"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
       <c r="D158" s="2"/>

</xml_diff>

<commit_message>
[FEATURE] Add test case for japanese language.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/configuration.xlsx
+++ b/Assets/StreamingAssets/configuration.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Korean</t>
   </si>
   <si>
+    <t xml:space="preserve">Japanese</t>
+  </si>
+  <si>
     <t xml:space="preserve">my.test.key1</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t xml:space="preserve">등록하십시오 </t>
   </si>
   <si>
+    <t xml:space="preserve">素敵な山 </t>
+  </si>
+  <si>
     <t xml:space="preserve">my.test.key2</t>
   </si>
   <si>
@@ -67,6 +73,9 @@
     <t xml:space="preserve">회의에서는 </t>
   </si>
   <si>
+    <t xml:space="preserve">最高のシチュー </t>
+  </si>
+  <si>
     <t xml:space="preserve">my.test.key3</t>
   </si>
   <si>
@@ -80,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">국제화와 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">めんつゆ </t>
   </si>
   <si>
     <t xml:space="preserve">my.test.key4</t>
@@ -117,7 +129,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -154,6 +166,12 @@
       <name val="Microsoft YaHei"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Mono;Courier New;DejaVu Sans Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -211,7 +229,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,6 +243,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -269,13 +291,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.21"/>
@@ -301,98 +323,110 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
@@ -466,45 +500,45 @@
       <c r="C25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4"/>
+      <c r="A26" s="5"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4"/>
+      <c r="A27" s="5"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4"/>
+      <c r="A28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4"/>
+      <c r="A29" s="5"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4"/>
+      <c r="A30" s="5"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4"/>
+      <c r="A31" s="5"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4"/>
+      <c r="A32" s="5"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4"/>
+      <c r="A33" s="5"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4"/>
+      <c r="A34" s="5"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
@@ -546,32 +580,32 @@
     <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6"/>
+      <c r="A56" s="7"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4"/>
+      <c r="A57" s="5"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="4"/>
+      <c r="A58" s="5"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="4"/>
+      <c r="A59" s="5"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="4"/>
+      <c r="A60" s="5"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="4"/>
+      <c r="A61" s="5"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
@@ -624,7 +658,7 @@
       <c r="C84" s="2"/>
     </row>
     <row r="85" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4"/>
+      <c r="A85" s="5"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
     </row>
@@ -634,7 +668,7 @@
     <row r="89" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="90" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C91" s="7"/>
+      <c r="C91" s="8"/>
     </row>
     <row r="92" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="93" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -669,30 +703,30 @@
     <row r="106" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="107" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="108" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="8"/>
+      <c r="A108" s="9"/>
     </row>
     <row r="109" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="4"/>
+      <c r="A109" s="5"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
     </row>
     <row r="110" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="4"/>
+      <c r="A110" s="5"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
     </row>
     <row r="111" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="4"/>
+      <c r="A111" s="5"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
     </row>
     <row r="112" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="4"/>
+      <c r="A112" s="5"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
     </row>
     <row r="113" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="4"/>
+      <c r="A113" s="5"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
     </row>
@@ -714,42 +748,42 @@
     <row r="125" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="126" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="127" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="4"/>
+      <c r="A127" s="5"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
     </row>
     <row r="128" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="4"/>
+      <c r="A128" s="5"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
     </row>
     <row r="129" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="4"/>
+      <c r="A129" s="5"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
     </row>
     <row r="130" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="4"/>
+      <c r="A130" s="5"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
     </row>
     <row r="131" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="4"/>
+      <c r="A131" s="5"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
     </row>
     <row r="132" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="4"/>
+      <c r="A132" s="5"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
     </row>
     <row r="133" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="4"/>
+      <c r="A133" s="5"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
     </row>
     <row r="134" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="4"/>
+      <c r="A134" s="5"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
     </row>
@@ -799,11 +833,11 @@
     <row r="154" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="155" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="156" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A156" s="9"/>
+      <c r="A156" s="10"/>
     </row>
     <row r="157" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="158" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="4"/>
+      <c r="A158" s="5"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
     </row>
@@ -1651,7 +1685,7 @@
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>